<commit_message>
Terminar las listas de componentes de ambos vendedores
</commit_message>
<xml_diff>
--- a/Conversor/Compra Componentes/Componentes DICOMSE.xlsx
+++ b/Conversor/Compra Componentes/Componentes DICOMSE.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t xml:space="preserve">Capacitores</t>
   </si>
@@ -107,19 +107,15 @@
   <si>
     <t xml:space="preserve">THT P2.54mm</t>
   </si>
-  <si>
-    <t xml:space="preserve">Conector jack</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -157,14 +153,8 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,14 +179,8 @@
         <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -214,15 +198,8 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
       <top/>
-      <bottom/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -251,7 +228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -329,38 +306,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,15 +397,15 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.71"/>
@@ -495,9 +448,6 @@
       <c r="D3" s="8" t="n">
         <v>3528</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>1061.77</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
@@ -540,9 +490,6 @@
       <c r="D7" s="14" t="n">
         <v>2512</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <v>726</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
@@ -585,9 +532,6 @@
       <c r="D11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="0" t="n">
-        <v>82.88</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
@@ -601,9 +545,6 @@
       </c>
       <c r="D12" s="16" t="s">
         <v>15</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>1193.4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -647,9 +588,6 @@
       <c r="D16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="0" t="n">
-        <v>248.62</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
@@ -663,9 +601,6 @@
       </c>
       <c r="D17" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>1989</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -709,9 +644,6 @@
       <c r="D21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="0" t="n">
-        <v>2386.8</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9"/>
@@ -742,42 +674,25 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="21" t="n">
+      <c r="C25" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="0" t="n">
-        <v>755.04</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="25" t="n">
-        <v>2</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>13</v>
-      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D27" s="9"/>
-      <c r="E27" s="27" t="n">
-        <f aca="false">SUM(E3:E26)</f>
-        <v>8443.51</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D28" s="9"/>
@@ -3620,9 +3535,7 @@
     <row r="974" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D974" s="9"/>
     </row>
-    <row r="975" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D975" s="9"/>
-    </row>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3678,7 +3591,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="10.71"/>
   </cols>
@@ -4685,7 +4598,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="10.71"/>
   </cols>

</xml_diff>

<commit_message>
Comprobar los componentes y empezar a soldar
</commit_message>
<xml_diff>
--- a/Conversor/Compra Componentes/Componentes DICOMSE.xlsx
+++ b/Conversor/Compra Componentes/Componentes DICOMSE.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t xml:space="preserve">Capacitores</t>
   </si>
@@ -48,52 +48,13 @@
     <t xml:space="preserve">Resistencias</t>
   </si>
   <si>
-    <t xml:space="preserve">Resistencia SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.004 (1%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Diodos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1N4148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAS40-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT-23</t>
   </si>
   <si>
     <t xml:space="preserve">Transistores</t>
   </si>
   <si>
-    <t xml:space="preserve">MMBT3904</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD SOT-23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRF7425</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOIC-8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Circuitos integrados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FT232BL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LQFP-32</t>
   </si>
   <si>
     <t xml:space="preserve">Otros</t>
@@ -228,7 +189,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,32 +238,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -397,10 +338,10 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
@@ -478,73 +419,59 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" s="14" t="n">
-        <v>2512</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="17" t="n">
-        <v>6</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -555,7 +482,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -576,120 +503,68 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>17</v>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>11</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="13" t="n">
-        <v>5</v>
+      <c r="B19" s="13" t="s">
+        <v>13</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="19" t="n">
+      <c r="C19" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>27</v>
+      <c r="D19" s="15" t="s">
+        <v>14</v>
       </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D20" s="9"/>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D26" s="9"/>
-      <c r="E26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D27" s="9"/>
@@ -3517,24 +3392,12 @@
     <row r="968" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D968" s="9"/>
     </row>
-    <row r="969" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D969" s="9"/>
-    </row>
-    <row r="970" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D970" s="9"/>
-    </row>
-    <row r="971" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D971" s="9"/>
-    </row>
-    <row r="972" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D972" s="9"/>
-    </row>
-    <row r="973" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D973" s="9"/>
-    </row>
-    <row r="974" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D974" s="9"/>
-    </row>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3565,10 +3428,10 @@
   <mergeCells count="6">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A11:D11"/>
     <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A17:D17"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3591,7 +3454,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="10.71"/>
   </cols>
@@ -4598,7 +4461,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="10.71"/>
   </cols>

</xml_diff>